<commit_message>
Cleanup and added latest 0.92.9 version of Repetier Firmware
</commit_message>
<xml_diff>
--- a/Firmware/P802M_8_Repetier_Thermistor_Tables.xlsx
+++ b/Firmware/P802M_8_Repetier_Thermistor_Tables.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perivar.nerseth\Documents\My Projects\PulpitRockCNC3D\Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perner\My Projects\PulpitRockCNC3D\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33443E3-8DD7-4D59-9BE5-F8257FBDF92F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="13335"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thermistor Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Reverse Engineer Repetier Table" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>R1</t>
   </si>
@@ -39,16 +46,10 @@
     <t>USER_THERMISTORTABLE0</t>
   </si>
   <si>
-    <t>USER_THERMISTORTABLE1</t>
-  </si>
-  <si>
     <t>{{1384,448},{1595,472},{1883,512}}</t>
   </si>
   <si>
     <t>{{1222,448},{1595,1496},{1883,4920},{2003,5520}}</t>
-  </si>
-  <si>
-    <t>Marlin Table</t>
   </si>
   <si>
     <t>ADC</t>
@@ -62,11 +63,23 @@
   <si>
     <t>ADC*4</t>
   </si>
+  <si>
+    <t>USER_THERMISTORTABLE1 (BED)</t>
+  </si>
+  <si>
+    <t>Marlin Table (temptable_501: 100k Zonestar thermistor. Adjusted By Hally)</t>
+  </si>
+  <si>
+    <t>OV(X)</t>
+  </si>
+  <si>
+    <t>Marlin OV(X)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,31 +447,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="5" max="5" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,11 +483,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -480,73 +495,95 @@
         <v>4700</v>
       </c>
       <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F3">
         <v>56</v>
       </c>
       <c r="G3">
+        <f>F3/4</f>
+        <v>14</v>
+      </c>
+      <c r="H3">
         <f>300*8</f>
         <v>2400</v>
       </c>
-      <c r="H3">
-        <f>G3/8</f>
+      <c r="I3">
+        <f>H3/8</f>
         <v>300</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>56</v>
       </c>
-      <c r="K3">
+      <c r="L3">
+        <f>K3/4</f>
+        <v>14</v>
+      </c>
+      <c r="M3">
         <f>300*8</f>
         <v>2400</v>
       </c>
-      <c r="L3">
-        <f>K3/8</f>
+      <c r="N3">
+        <f>M3/8</f>
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F4">
         <v>59</v>
       </c>
       <c r="G4">
+        <f>F4/4</f>
+        <v>14.75</v>
+      </c>
+      <c r="H4">
         <f>295*8</f>
         <v>2360</v>
       </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H60" si="0">G4/8</f>
+      <c r="I4">
+        <f t="shared" ref="I4:I60" si="0">H4/8</f>
         <v>295</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>187</v>
       </c>
-      <c r="K4">
+      <c r="L4">
+        <f t="shared" ref="L4:L35" si="1">K4/4</f>
+        <v>46.75</v>
+      </c>
+      <c r="M4">
         <f>250*8</f>
         <v>2000</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L35" si="1">K4/8</f>
+      <c r="N4">
+        <f t="shared" ref="N4:N35" si="2">M4/8</f>
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>56</v>
       </c>
@@ -557,32 +594,40 @@
         <v>1384.2253521127</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>64</v>
       </c>
       <c r="G5">
+        <f>F5/4</f>
+        <v>16</v>
+      </c>
+      <c r="H5">
         <f>290*8</f>
         <v>2320</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>615</v>
       </c>
-      <c r="K5">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>153.75</v>
+      </c>
+      <c r="M5">
         <f>190*8</f>
         <v>1520</v>
       </c>
-      <c r="L5">
-        <f t="shared" si="1"/>
+      <c r="N5">
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>59</v>
       </c>
@@ -596,26 +641,34 @@
         <v>70</v>
       </c>
       <c r="G6">
+        <f>F6/4</f>
+        <v>17.5</v>
+      </c>
+      <c r="H6">
         <f>285*8</f>
         <v>2280</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>285</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>690</v>
       </c>
-      <c r="K6">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>172.5</v>
+      </c>
+      <c r="M6">
         <f>185*8</f>
         <v>1480</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
+      <c r="N6">
+        <f t="shared" si="2"/>
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>64</v>
       </c>
@@ -629,50 +682,66 @@
         <v>76</v>
       </c>
       <c r="G7">
+        <f>F7/4</f>
+        <v>19</v>
+      </c>
+      <c r="H7">
         <f>280*8</f>
         <v>2240</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>280</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>750</v>
       </c>
-      <c r="K7">
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>187.5</v>
+      </c>
+      <c r="M7">
         <f>180*8</f>
         <v>1440</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
+      <c r="N7">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F8">
         <v>82</v>
       </c>
       <c r="G8">
+        <f t="shared" ref="G8:G60" si="3">F8/4</f>
+        <v>20.5</v>
+      </c>
+      <c r="H8">
         <f>275*8</f>
         <v>2200</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>275</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>830</v>
       </c>
-      <c r="K8">
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>207.5</v>
+      </c>
+      <c r="M8">
         <f>175*8</f>
         <v>1400</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
+      <c r="N8">
+        <f t="shared" si="2"/>
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>56</v>
       </c>
@@ -683,32 +752,40 @@
         <v>1222.3880597015</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>89</v>
       </c>
       <c r="G9">
+        <f t="shared" si="3"/>
+        <v>22.25</v>
+      </c>
+      <c r="H9">
         <f>270*8</f>
         <v>2160</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>920</v>
       </c>
-      <c r="K9">
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="M9">
         <f>170*8</f>
         <v>1360</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
+      <c r="N9">
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>187</v>
       </c>
@@ -722,26 +799,34 @@
         <v>98</v>
       </c>
       <c r="G10">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="H10">
         <f>265*8</f>
         <v>2120</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1010</v>
       </c>
-      <c r="K10">
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>252.5</v>
+      </c>
+      <c r="M10">
         <f>165*8</f>
         <v>1320</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
+      <c r="N10">
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>615</v>
       </c>
@@ -755,26 +840,34 @@
         <v>108</v>
       </c>
       <c r="G11">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="H11">
         <f>260*8</f>
         <v>2080</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>260</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1118</v>
       </c>
-      <c r="K11">
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>279.5</v>
+      </c>
+      <c r="M11">
         <f>160*8</f>
         <v>1280</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
+      <c r="N11">
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>690</v>
       </c>
@@ -788,112 +881,147 @@
         <v>118</v>
       </c>
       <c r="G12">
+        <f t="shared" si="3"/>
+        <v>29.5</v>
+      </c>
+      <c r="H12">
         <f>255*8</f>
         <v>2040</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>255</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1215</v>
       </c>
-      <c r="K12">
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>303.75</v>
+      </c>
+      <c r="M12">
         <f>155*8</f>
         <v>1240</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
+      <c r="N12">
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F13">
         <v>128</v>
       </c>
       <c r="G13">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="H13">
         <f>250*8</f>
         <v>2000</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1330</v>
       </c>
-      <c r="K13">
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>332.5</v>
+      </c>
+      <c r="M13">
         <f>145*8</f>
         <v>1160</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
+      <c r="N13">
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F14">
         <v>145</v>
       </c>
       <c r="G14">
+        <f t="shared" si="3"/>
+        <v>36.25</v>
+      </c>
+      <c r="H14">
         <f>245*8</f>
         <v>1960</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1460</v>
       </c>
-      <c r="K14">
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
+      <c r="M14">
         <f>140*8</f>
         <v>1120</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
+      <c r="N14">
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
         <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
       </c>
       <c r="F15">
         <v>156</v>
       </c>
       <c r="G15">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="H15">
         <f>240*8</f>
         <v>1920</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1594</v>
       </c>
-      <c r="K15">
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>398.5</v>
+      </c>
+      <c r="M15">
         <f>135*8</f>
         <v>1080</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
+      <c r="N15">
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f>B16/4</f>
+        <f>C16*4</f>
         <v>4</v>
       </c>
       <c r="B16">
@@ -901,34 +1029,46 @@
         <v>16</v>
       </c>
       <c r="C16">
+        <f>B16/16</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>713</v>
       </c>
       <c r="F16">
         <v>168</v>
       </c>
       <c r="G16">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="H16">
         <f>235*8</f>
         <v>1880</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1752</v>
       </c>
-      <c r="K16">
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>438</v>
+      </c>
+      <c r="M16">
         <f>130*8</f>
         <v>1040</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
+      <c r="N16">
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f>B17/4</f>
+        <f>C17*4</f>
         <v>56</v>
       </c>
       <c r="B17">
@@ -936,34 +1076,46 @@
         <v>224</v>
       </c>
       <c r="C17">
+        <f t="shared" ref="C17:C47" si="4">B17/16</f>
+        <v>14</v>
+      </c>
+      <c r="D17">
         <v>300</v>
       </c>
       <c r="F17">
         <v>187</v>
       </c>
       <c r="G17">
+        <f t="shared" si="3"/>
+        <v>46.75</v>
+      </c>
+      <c r="H17">
         <f>230*8</f>
         <v>1840</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1900</v>
       </c>
-      <c r="K17">
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>475</v>
+      </c>
+      <c r="M17">
         <f>125*8</f>
         <v>1000</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
+      <c r="N17">
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f>B18/4</f>
+        <f>C18*4</f>
         <v>64</v>
       </c>
       <c r="B18">
@@ -971,34 +1123,46 @@
         <v>256</v>
       </c>
       <c r="C18">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="D18">
         <v>290</v>
       </c>
       <c r="F18">
         <v>208</v>
       </c>
       <c r="G18">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="H18">
         <f>225*8</f>
         <v>1800</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>2040</v>
       </c>
-      <c r="K18">
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>510</v>
+      </c>
+      <c r="M18">
         <f>120*8</f>
         <v>960</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
+      <c r="N18">
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f>B19/4</f>
+        <f t="shared" ref="A19:A47" si="5">C19*4</f>
         <v>76</v>
       </c>
       <c r="B19">
@@ -1006,34 +1170,46 @@
         <v>304</v>
       </c>
       <c r="C19">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="D19">
         <v>280</v>
       </c>
       <c r="F19">
         <v>227</v>
       </c>
       <c r="G19">
+        <f t="shared" si="3"/>
+        <v>56.75</v>
+      </c>
+      <c r="H19">
         <f>220*8</f>
         <v>1760</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>2200</v>
       </c>
-      <c r="K19">
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="M19">
         <f>115*8</f>
         <v>920</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
+      <c r="N19">
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f>B20/4</f>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="B20">
@@ -1041,34 +1217,46 @@
         <v>368</v>
       </c>
       <c r="C20">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="D20">
         <v>270</v>
       </c>
       <c r="F20">
         <v>248</v>
       </c>
       <c r="G20">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="H20">
         <f>215*8</f>
         <v>1720</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>2350</v>
       </c>
-      <c r="K20">
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>587.5</v>
+      </c>
+      <c r="M20">
         <f>110*8</f>
         <v>880</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
+      <c r="N20">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f>B21/4</f>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="B21">
@@ -1076,34 +1264,46 @@
         <v>432</v>
       </c>
       <c r="C21">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="D21">
         <v>260</v>
       </c>
       <c r="F21">
         <v>272</v>
       </c>
       <c r="G21">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="H21">
         <f>210*8</f>
         <v>1680</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>2516</v>
       </c>
-      <c r="K21">
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>629</v>
+      </c>
+      <c r="M21">
         <f>105*8</f>
         <v>840</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="1"/>
+      <c r="N21">
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
-        <f>B22/4</f>
+        <f t="shared" si="5"/>
         <v>124</v>
       </c>
       <c r="B22">
@@ -1111,34 +1311,46 @@
         <v>496</v>
       </c>
       <c r="C22">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="D22">
         <v>250</v>
       </c>
       <c r="F22">
         <v>301</v>
       </c>
       <c r="G22">
+        <f t="shared" si="3"/>
+        <v>75.25</v>
+      </c>
+      <c r="H22">
         <f>205*8</f>
         <v>1640</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>205</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2671</v>
       </c>
-      <c r="K22">
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>667.75</v>
+      </c>
+      <c r="M22">
         <f>98*8</f>
         <v>784</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="1"/>
+      <c r="N22">
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
-        <f>B23/4</f>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="B23">
@@ -1146,34 +1358,46 @@
         <v>592</v>
       </c>
       <c r="C23">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="D23">
         <v>240</v>
       </c>
       <c r="F23">
         <v>336</v>
       </c>
       <c r="G23">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="H23">
         <f>200*8</f>
         <v>1600</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>2831</v>
       </c>
-      <c r="K23">
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>707.75</v>
+      </c>
+      <c r="M23">
         <f>92*8</f>
         <v>736</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="1"/>
+      <c r="N23">
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
-        <f>B24/4</f>
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="B24">
@@ -1181,34 +1405,46 @@
         <v>752</v>
       </c>
       <c r="C24">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="D24">
         <v>230</v>
       </c>
       <c r="F24">
         <v>370</v>
       </c>
       <c r="G24">
+        <f t="shared" si="3"/>
+        <v>92.5</v>
+      </c>
+      <c r="H24">
         <f>195*8</f>
         <v>1560</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f t="shared" si="0"/>
         <v>195</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>2975</v>
       </c>
-      <c r="K24">
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>743.75</v>
+      </c>
+      <c r="M24">
         <f>85*8</f>
         <v>680</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
+      <c r="N24">
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
-        <f>B25/4</f>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="B25">
@@ -1216,34 +1452,46 @@
         <v>912</v>
       </c>
       <c r="C25">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="D25">
         <v>220</v>
       </c>
       <c r="F25">
         <v>400</v>
       </c>
       <c r="G25">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H25">
         <f>190*8</f>
         <v>1520</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>3115</v>
       </c>
-      <c r="K25">
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>778.75</v>
+      </c>
+      <c r="M25">
         <f>76*8</f>
         <v>608</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="1"/>
+      <c r="N25">
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
-        <f>B26/4</f>
+        <f t="shared" si="5"/>
         <v>272</v>
       </c>
       <c r="B26">
@@ -1251,34 +1499,46 @@
         <v>1088</v>
       </c>
       <c r="C26">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="D26">
         <v>210</v>
       </c>
       <c r="F26">
         <v>450</v>
       </c>
       <c r="G26">
+        <f t="shared" si="3"/>
+        <v>112.5</v>
+      </c>
+      <c r="H26">
         <f>185*8</f>
         <v>1480</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>185</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>3251</v>
       </c>
-      <c r="K26">
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>812.75</v>
+      </c>
+      <c r="M26">
         <f>72*8</f>
         <v>576</v>
       </c>
-      <c r="L26">
-        <f t="shared" si="1"/>
+      <c r="N26">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
-        <f>B27/4</f>
+        <f t="shared" si="5"/>
         <v>336</v>
       </c>
       <c r="B27">
@@ -1286,34 +1546,46 @@
         <v>1344</v>
       </c>
       <c r="C27">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="D27">
         <v>200</v>
       </c>
       <c r="F27">
         <v>492</v>
       </c>
       <c r="G27">
+        <f t="shared" si="3"/>
+        <v>123</v>
+      </c>
+      <c r="H27">
         <f>180*8</f>
         <v>1440</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>3480</v>
       </c>
-      <c r="K27">
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="M27">
         <f>62*8</f>
         <v>496</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="1"/>
+      <c r="N27">
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
-        <f>B28/4</f>
+        <f t="shared" si="5"/>
         <v>400</v>
       </c>
       <c r="B28">
@@ -1321,34 +1593,46 @@
         <v>1600</v>
       </c>
       <c r="C28">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="D28">
         <v>190</v>
       </c>
       <c r="F28">
         <v>552</v>
       </c>
       <c r="G28">
+        <f t="shared" si="3"/>
+        <v>138</v>
+      </c>
+      <c r="H28">
         <f>175*8</f>
         <v>1400</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>3580</v>
       </c>
-      <c r="K28">
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>895</v>
+      </c>
+      <c r="M28">
         <f>52*8</f>
         <v>416</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="1"/>
+      <c r="N28">
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
-        <f>B29/4</f>
+        <f t="shared" si="5"/>
         <v>512</v>
       </c>
       <c r="B29">
@@ -1356,34 +1640,46 @@
         <v>2048</v>
       </c>
       <c r="C29">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="D29">
         <v>180</v>
       </c>
       <c r="F29">
         <v>615</v>
       </c>
       <c r="G29">
+        <f t="shared" si="3"/>
+        <v>153.75</v>
+      </c>
+      <c r="H29">
         <f>170*8</f>
         <v>1360</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>3660</v>
       </c>
-      <c r="K29">
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>915</v>
+      </c>
+      <c r="M29">
         <f>46*8</f>
         <v>368</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="1"/>
+      <c r="N29">
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
-        <f>B30/4</f>
+        <f t="shared" si="5"/>
         <v>620</v>
       </c>
       <c r="B30">
@@ -1391,34 +1687,46 @@
         <v>2480</v>
       </c>
       <c r="C30">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
+      <c r="D30">
         <v>170</v>
       </c>
       <c r="F30">
         <v>690</v>
       </c>
       <c r="G30">
+        <f t="shared" si="3"/>
+        <v>172.5</v>
+      </c>
+      <c r="H30">
         <f>165*8</f>
         <v>1320</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>3740</v>
       </c>
-      <c r="K30">
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>935</v>
+      </c>
+      <c r="M30">
         <f>40*8</f>
         <v>320</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="1"/>
+      <c r="N30">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
-        <f>B31/4</f>
+        <f t="shared" si="5"/>
         <v>756</v>
       </c>
       <c r="B31">
@@ -1426,34 +1734,46 @@
         <v>3024</v>
       </c>
       <c r="C31">
+        <f t="shared" si="4"/>
+        <v>189</v>
+      </c>
+      <c r="D31">
         <v>160</v>
       </c>
       <c r="F31">
         <v>750</v>
       </c>
       <c r="G31">
+        <f t="shared" si="3"/>
+        <v>187.5</v>
+      </c>
+      <c r="H31">
         <f>160*8</f>
         <v>1280</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>3869</v>
       </c>
-      <c r="K31">
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>967.25</v>
+      </c>
+      <c r="M31">
         <f>30*8</f>
         <v>240</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="1"/>
+      <c r="N31">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
-        <f>B32/4</f>
+        <f t="shared" si="5"/>
         <v>920</v>
       </c>
       <c r="B32">
@@ -1461,34 +1781,46 @@
         <v>3680</v>
       </c>
       <c r="C32">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="D32">
         <v>150</v>
       </c>
       <c r="F32">
         <v>830</v>
       </c>
       <c r="G32">
+        <f t="shared" si="3"/>
+        <v>207.5</v>
+      </c>
+      <c r="H32">
         <f>155*8</f>
         <v>1240</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>3912</v>
       </c>
-      <c r="K32">
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>978</v>
+      </c>
+      <c r="M32">
         <f>25*8</f>
         <v>200</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="1"/>
+      <c r="N32">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
-        <f>B33/4</f>
+        <f t="shared" si="5"/>
         <v>1112</v>
       </c>
       <c r="B33">
@@ -1496,34 +1828,46 @@
         <v>4448</v>
       </c>
       <c r="C33">
+        <f t="shared" si="4"/>
+        <v>278</v>
+      </c>
+      <c r="D33">
         <v>140</v>
       </c>
       <c r="F33">
         <v>920</v>
       </c>
       <c r="G33">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="H33">
         <f>150*8</f>
         <v>1200</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>3948</v>
       </c>
-      <c r="K33">
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>987</v>
+      </c>
+      <c r="M33">
         <f>20*8</f>
         <v>160</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="1"/>
+      <c r="N33">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
-        <f>B34/4</f>
+        <f t="shared" si="5"/>
         <v>1344</v>
       </c>
       <c r="B34">
@@ -1531,34 +1875,46 @@
         <v>5376</v>
       </c>
       <c r="C34">
+        <f t="shared" si="4"/>
+        <v>336</v>
+      </c>
+      <c r="D34">
         <v>130</v>
       </c>
       <c r="F34">
         <v>1010</v>
       </c>
       <c r="G34">
+        <f t="shared" si="3"/>
+        <v>252.5</v>
+      </c>
+      <c r="H34">
         <f>145*8</f>
         <v>1160</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>4077</v>
       </c>
-      <c r="K34">
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>1019.25</v>
+      </c>
+      <c r="M34">
         <f>-20*8</f>
         <v>-160</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="1"/>
+      <c r="N34">
+        <f t="shared" si="2"/>
         <v>-20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
-        <f>B35/4</f>
+        <f t="shared" si="5"/>
         <v>1608</v>
       </c>
       <c r="B35">
@@ -1566,34 +1922,46 @@
         <v>6432</v>
       </c>
       <c r="C35">
+        <f t="shared" si="4"/>
+        <v>402</v>
+      </c>
+      <c r="D35">
         <v>120</v>
       </c>
       <c r="F35">
         <v>1118</v>
       </c>
       <c r="G35">
+        <f t="shared" si="3"/>
+        <v>279.5</v>
+      </c>
+      <c r="H35">
         <f>140*8</f>
         <v>1120</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>4094</v>
       </c>
-      <c r="K35">
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>1023.5</v>
+      </c>
+      <c r="M35">
         <f>-55*8</f>
         <v>-440</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="1"/>
+      <c r="N35">
+        <f t="shared" si="2"/>
         <v>-55</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
-        <f>B36/4</f>
+        <f t="shared" si="5"/>
         <v>1904</v>
       </c>
       <c r="B36">
@@ -1601,23 +1969,31 @@
         <v>7616</v>
       </c>
       <c r="C36">
+        <f t="shared" si="4"/>
+        <v>476</v>
+      </c>
+      <c r="D36">
         <v>110</v>
       </c>
       <c r="F36">
         <v>1215</v>
       </c>
       <c r="G36">
+        <f t="shared" si="3"/>
+        <v>303.75</v>
+      </c>
+      <c r="H36">
         <f>135*8</f>
         <v>1080</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f>B37/4</f>
+        <f t="shared" si="5"/>
         <v>2216</v>
       </c>
       <c r="B37">
@@ -1625,23 +2001,31 @@
         <v>8864</v>
       </c>
       <c r="C37">
+        <f t="shared" si="4"/>
+        <v>554</v>
+      </c>
+      <c r="D37">
         <v>100</v>
       </c>
       <c r="F37">
         <v>1330</v>
       </c>
       <c r="G37">
+        <f t="shared" si="3"/>
+        <v>332.5</v>
+      </c>
+      <c r="H37">
         <f>130*8</f>
         <v>1040</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f>B38/4</f>
+        <f t="shared" si="5"/>
         <v>2540</v>
       </c>
       <c r="B38">
@@ -1649,23 +2033,31 @@
         <v>10160</v>
       </c>
       <c r="C38">
+        <f t="shared" si="4"/>
+        <v>635</v>
+      </c>
+      <c r="D38">
         <v>90</v>
       </c>
       <c r="F38">
         <v>1460</v>
       </c>
       <c r="G38">
+        <f t="shared" si="3"/>
+        <v>365</v>
+      </c>
+      <c r="H38">
         <f>125*8</f>
         <v>1000</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f>B39/4</f>
+        <f t="shared" si="5"/>
         <v>2852</v>
       </c>
       <c r="B39">
@@ -1673,23 +2065,31 @@
         <v>11408</v>
       </c>
       <c r="C39">
+        <f t="shared" si="4"/>
+        <v>713</v>
+      </c>
+      <c r="D39">
         <v>80</v>
       </c>
       <c r="F39">
         <v>1594</v>
       </c>
       <c r="G39">
+        <f t="shared" si="3"/>
+        <v>398.5</v>
+      </c>
+      <c r="H39">
         <f>120*8</f>
         <v>960</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f>B40/4</f>
+        <f t="shared" si="5"/>
         <v>3136</v>
       </c>
       <c r="B40">
@@ -1697,23 +2097,31 @@
         <v>12544</v>
       </c>
       <c r="C40">
+        <f t="shared" si="4"/>
+        <v>784</v>
+      </c>
+      <c r="D40">
         <v>70</v>
       </c>
       <c r="F40">
         <v>1752</v>
       </c>
       <c r="G40">
+        <f t="shared" si="3"/>
+        <v>438</v>
+      </c>
+      <c r="H40">
         <f>115*8</f>
         <v>920</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41">
-        <f>B41/4</f>
+        <f t="shared" si="5"/>
         <v>3384</v>
       </c>
       <c r="B41">
@@ -1721,23 +2129,31 @@
         <v>13536</v>
       </c>
       <c r="C41">
+        <f t="shared" si="4"/>
+        <v>846</v>
+      </c>
+      <c r="D41">
         <v>60</v>
       </c>
       <c r="F41">
         <v>1900</v>
       </c>
       <c r="G41">
+        <f t="shared" si="3"/>
+        <v>475</v>
+      </c>
+      <c r="H41">
         <f>110*8</f>
         <v>880</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42">
-        <f>B42/4</f>
+        <f t="shared" si="5"/>
         <v>3588</v>
       </c>
       <c r="B42">
@@ -1745,23 +2161,31 @@
         <v>14352</v>
       </c>
       <c r="C42">
+        <f t="shared" si="4"/>
+        <v>897</v>
+      </c>
+      <c r="D42">
         <v>50</v>
       </c>
       <c r="F42">
         <v>2040</v>
       </c>
       <c r="G42">
+        <f t="shared" si="3"/>
+        <v>510</v>
+      </c>
+      <c r="H42">
         <f>105*8</f>
         <v>840</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43">
-        <f>B43/4</f>
+        <f t="shared" si="5"/>
         <v>3748</v>
       </c>
       <c r="B43">
@@ -1769,23 +2193,31 @@
         <v>14992</v>
       </c>
       <c r="C43">
+        <f t="shared" si="4"/>
+        <v>937</v>
+      </c>
+      <c r="D43">
         <v>40</v>
       </c>
       <c r="F43">
         <v>2200</v>
       </c>
       <c r="G43">
+        <f t="shared" si="3"/>
+        <v>550</v>
+      </c>
+      <c r="H43">
         <f>100*8</f>
         <v>800</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44">
-        <f>B44/4</f>
+        <f t="shared" si="5"/>
         <v>3864</v>
       </c>
       <c r="B44">
@@ -1793,23 +2225,31 @@
         <v>15456</v>
       </c>
       <c r="C44">
+        <f t="shared" si="4"/>
+        <v>966</v>
+      </c>
+      <c r="D44">
         <v>30</v>
       </c>
       <c r="F44">
         <v>2350</v>
       </c>
       <c r="G44">
+        <f t="shared" si="3"/>
+        <v>587.5</v>
+      </c>
+      <c r="H44">
         <f>95*8</f>
         <v>760</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45">
-        <f>B45/4</f>
+        <f t="shared" si="5"/>
         <v>3944</v>
       </c>
       <c r="B45">
@@ -1817,23 +2257,31 @@
         <v>15776</v>
       </c>
       <c r="C45">
+        <f t="shared" si="4"/>
+        <v>986</v>
+      </c>
+      <c r="D45">
         <v>20</v>
       </c>
       <c r="F45">
         <v>2516</v>
       </c>
       <c r="G45">
+        <f t="shared" si="3"/>
+        <v>629</v>
+      </c>
+      <c r="H45">
         <f>90*8</f>
         <v>720</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46">
-        <f>B46/4</f>
+        <f t="shared" si="5"/>
         <v>4000</v>
       </c>
       <c r="B46">
@@ -1841,23 +2289,31 @@
         <v>16000</v>
       </c>
       <c r="C46">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="D46">
         <v>10</v>
       </c>
       <c r="F46">
         <v>2671</v>
       </c>
       <c r="G46">
+        <f t="shared" si="3"/>
+        <v>667.75</v>
+      </c>
+      <c r="H46">
         <f>85*8</f>
         <v>680</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47">
-        <f>B47/4</f>
+        <f t="shared" si="5"/>
         <v>4040</v>
       </c>
       <c r="B47">
@@ -1865,185 +2321,245 @@
         <v>16160</v>
       </c>
       <c r="C47">
+        <f t="shared" si="4"/>
+        <v>1010</v>
+      </c>
+      <c r="D47">
         <v>0</v>
       </c>
       <c r="F47">
         <v>2831</v>
       </c>
       <c r="G47">
+        <f t="shared" si="3"/>
+        <v>707.75</v>
+      </c>
+      <c r="H47">
         <f>80*8</f>
         <v>640</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F48">
         <v>2975</v>
       </c>
       <c r="G48">
+        <f t="shared" si="3"/>
+        <v>743.75</v>
+      </c>
+      <c r="H48">
         <f>75*8</f>
         <v>600</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F49">
         <v>3115</v>
       </c>
       <c r="G49">
+        <f t="shared" si="3"/>
+        <v>778.75</v>
+      </c>
+      <c r="H49">
         <f>70*8</f>
         <v>560</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F50">
         <v>3251</v>
       </c>
       <c r="G50">
+        <f t="shared" si="3"/>
+        <v>812.75</v>
+      </c>
+      <c r="H50">
         <f>65*8</f>
         <v>520</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F51">
         <v>3375</v>
       </c>
       <c r="G51">
+        <f t="shared" si="3"/>
+        <v>843.75</v>
+      </c>
+      <c r="H51">
         <f>60*8</f>
         <v>480</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F52">
         <v>3480</v>
       </c>
       <c r="G52">
+        <f t="shared" si="3"/>
+        <v>870</v>
+      </c>
+      <c r="H52">
         <f>55*8</f>
         <v>440</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F53">
         <v>3580</v>
       </c>
       <c r="G53">
+        <f t="shared" si="3"/>
+        <v>895</v>
+      </c>
+      <c r="H53">
         <f>50*8</f>
         <v>400</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F54">
         <v>3660</v>
       </c>
       <c r="G54">
+        <f t="shared" si="3"/>
+        <v>915</v>
+      </c>
+      <c r="H54">
         <f>45*8</f>
         <v>360</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F55">
         <v>3740</v>
       </c>
       <c r="G55">
+        <f t="shared" si="3"/>
+        <v>935</v>
+      </c>
+      <c r="H55">
         <f>40*8</f>
         <v>320</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F56">
         <v>3869</v>
       </c>
       <c r="G56">
+        <f t="shared" si="3"/>
+        <v>967.25</v>
+      </c>
+      <c r="H56">
         <f>30*8</f>
         <v>240</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F57">
         <v>3912</v>
       </c>
       <c r="G57">
+        <f t="shared" si="3"/>
+        <v>978</v>
+      </c>
+      <c r="H57">
         <f>25*8</f>
         <v>200</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F58">
         <v>3948</v>
       </c>
       <c r="G58">
+        <f t="shared" si="3"/>
+        <v>987</v>
+      </c>
+      <c r="H58">
         <f>20*8</f>
         <v>160</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F59">
         <v>4077</v>
       </c>
       <c r="G59">
+        <f t="shared" si="3"/>
+        <v>1019.25</v>
+      </c>
+      <c r="H59">
         <f>-20*8</f>
         <v>-160</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:9" x14ac:dyDescent="0.35">
       <c r="F60">
         <v>4094</v>
       </c>
       <c r="G60">
+        <f t="shared" si="3"/>
+        <v>1023.5</v>
+      </c>
+      <c r="H60">
         <f>-55*8</f>
         <v>-440</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <f t="shared" si="0"/>
         <v>-55</v>
       </c>
@@ -2054,16 +2570,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>4700</v>
       </c>
@@ -2071,7 +2587,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -2084,7 +2600,7 @@
         <v>1222.3880597014925</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2400</v>
       </c>
@@ -2097,7 +2613,7 @@
         <v>1384.2253521126761</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3000</v>
       </c>
@@ -2110,7 +2626,7 @@
         <v>1595.4545454545455</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4000</v>
       </c>
@@ -2123,7 +2639,7 @@
         <v>1882.7586206896551</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4500</v>
       </c>
@@ -2136,7 +2652,7 @@
         <v>2002.9891304347827</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>10</v>
       </c>
@@ -2149,7 +2665,7 @@
         <v>8.6942675159235669</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>C18</f>
         <v>65.164644714038133</v>
@@ -2163,7 +2679,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>C19</f>
         <v>68.706640237859261</v>
@@ -2177,7 +2693,7 @@
         <v>58.999999999999986</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>C20</f>
         <v>4665.6934306569347</v>
@@ -2191,7 +2707,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>C24</f>
         <v>39544.827586206899</v>
@@ -2205,7 +2721,7 @@
         <v>3660</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>C26</f>
         <v>1064550</v>
@@ -2219,7 +2735,7 @@
         <v>4077</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>C27</f>
         <v>19241800</v>
@@ -2233,7 +2749,7 @@
         <v>4094</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>56</v>
       </c>
@@ -2246,7 +2762,7 @@
         <v>65.164644714038133</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>59</v>
       </c>
@@ -2259,7 +2775,7 @@
         <v>68.706640237859261</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2040</v>
       </c>
@@ -2272,7 +2788,7 @@
         <v>4665.6934306569347</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2516</v>
       </c>
@@ -2285,7 +2801,7 @@
         <v>7489.0436985433817</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3115</v>
       </c>
@@ -2298,7 +2814,7 @@
         <v>14939.285714285714</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3480</v>
       </c>
@@ -2311,7 +2827,7 @@
         <v>26595.121951219513</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3660</v>
       </c>
@@ -2324,7 +2840,7 @@
         <v>39544.827586206899</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3912</v>
       </c>
@@ -2337,7 +2853,7 @@
         <v>100472.13114754099</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>4077</v>
       </c>
@@ -2350,7 +2866,7 @@
         <v>1064550</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>4094</v>
       </c>

</xml_diff>

<commit_message>
Modified the thermistor tables, updated the pulpit scad, added zonestar sd card contents and 3d models for upgrades to zonestar p802m
</commit_message>
<xml_diff>
--- a/Firmware/P802M_8_Repetier_Thermistor_Tables.xlsx
+++ b/Firmware/P802M_8_Repetier_Thermistor_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perner\My Projects\PulpitRockCNC3D\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33443E3-8DD7-4D59-9BE5-F8257FBDF92F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DDE9FA-930A-4CC7-B002-391960943781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -41,9 +43,6 @@
   </si>
   <si>
     <t>R2</t>
-  </si>
-  <si>
-    <t>USER_THERMISTORTABLE0</t>
   </si>
   <si>
     <t>{{1384,448},{1595,472},{1883,512}}</t>
@@ -74,6 +73,9 @@
   </si>
   <si>
     <t>Marlin OV(X)</t>
+  </si>
+  <si>
+    <t>USER_THERMISTORTABLE0 (Extruder)</t>
   </si>
 </sst>
 </file>
@@ -454,7 +456,7 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -495,28 +497,28 @@
         <v>4700</v>
       </c>
       <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
       <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>6</v>
-      </c>
-      <c r="N2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -594,7 +596,7 @@
         <v>1384.2253521127</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>64</v>
@@ -752,7 +754,7 @@
         <v>1222.3880597015</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <v>89</v>
@@ -942,7 +944,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>145</v>
@@ -977,16 +979,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15">
         <v>156</v>

</xml_diff>